<commit_message>
Edit show command nx_os
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luthfi.anandra.COMPNET\AppData\Local\Programs\Python\Python37\Lib\site-packages\netoprmgr\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D195BE-3E06-481D-B89B-93CF4DA0FF10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8207FFFD-3AE8-43A7-81BD-A5ACB716BEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="192">
   <si>
     <t>cisco_ios</t>
   </si>
@@ -583,6 +583,24 @@
   </si>
   <si>
     <t>show msglog</t>
+  </si>
+  <si>
+    <t>show vdc membership</t>
+  </si>
+  <si>
+    <t>show vdc current</t>
+  </si>
+  <si>
+    <t>show vdc resources</t>
+  </si>
+  <si>
+    <t>show vpc</t>
+  </si>
+  <si>
+    <t>show vcp role</t>
+  </si>
+  <si>
+    <t>show vpc peer-keepalive</t>
   </si>
 </sst>
 </file>
@@ -936,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="CO1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CO4" sqref="CO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1047,7 @@
     <col min="93" max="93" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="26" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="29" bestFit="1" customWidth="1"/>
@@ -1889,150 +1907,168 @@
         <v>143</v>
       </c>
       <c r="AQ4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>187</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>189</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>190</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW4" t="s">
         <v>144</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AX4" t="s">
         <v>145</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AY4" t="s">
         <v>146</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AZ4" t="s">
         <v>147</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="BA4" t="s">
         <v>148</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="BB4" t="s">
         <v>149</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="BC4" t="s">
         <v>150</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="BD4" t="s">
         <v>151</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BE4" t="s">
         <v>152</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BF4" t="s">
         <v>153</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BG4" t="s">
         <v>154</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BH4" t="s">
         <v>155</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BI4" t="s">
         <v>156</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BJ4" t="s">
         <v>157</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BK4" t="s">
         <v>158</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BL4" t="s">
         <v>43</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BM4" t="s">
         <v>159</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BN4" t="s">
         <v>160</v>
       </c>
-      <c r="BI4" t="s">
+      <c r="BO4" t="s">
         <v>161</v>
       </c>
-      <c r="BJ4" t="s">
+      <c r="BP4" t="s">
         <v>162</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BQ4" t="s">
         <v>163</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BR4" t="s">
         <v>86</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BS4" t="s">
         <v>164</v>
       </c>
-      <c r="BN4" t="s">
+      <c r="BT4" t="s">
         <v>98</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BU4" t="s">
         <v>97</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BV4" t="s">
         <v>84</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BW4" t="s">
         <v>75</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="BX4" t="s">
         <v>165</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="BY4" t="s">
         <v>166</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="BZ4" t="s">
         <v>167</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="CA4" t="s">
         <v>168</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="CB4" t="s">
         <v>169</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="CC4" t="s">
         <v>157</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="CD4" t="s">
         <v>170</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="CE4" t="s">
         <v>52</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CF4" t="s">
         <v>171</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CG4" t="s">
         <v>172</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CH4" t="s">
         <v>173</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CI4" t="s">
         <v>62</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CJ4" t="s">
         <v>63</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CK4" t="s">
         <v>64</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CL4" t="s">
         <v>65</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CM4" t="s">
         <v>66</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CN4" t="s">
         <v>67</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CO4" t="s">
         <v>174</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CP4" t="s">
         <v>175</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CQ4" t="s">
         <v>176</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CR4" t="s">
         <v>177</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CS4" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>